<commit_message>
Ajustando o Cronograma e o GPR, e deletando artefatos sobre mudança
Arrumando uma linha da tabela do cronograma, excluindo as partes que
falam sobre mudanças no Plano de Gerenciamento e no Processo GPR, bem
como apagando os templates Log de Mudança e Solicitação de Mudança.
</commit_message>
<xml_diff>
--- a/Artefatos de Documentação/Processo Genérico/2-Gerencia de Projeto/Templates/Cronograma.xlsx
+++ b/Artefatos de Documentação/Processo Genérico/2-Gerencia de Projeto/Templates/Cronograma.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Atividade</t>
   </si>
@@ -65,9 +65,6 @@
   </si>
   <si>
     <t>DeadLine</t>
-  </si>
-  <si>
-    <t>Pendências</t>
   </si>
   <si>
     <t>Breve descrição da atividade</t>
@@ -1793,7 +1790,7 @@
         <v>4</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
@@ -2215,7 +2212,7 @@
   <dimension ref="B1:C14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2234,7 +2231,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
@@ -2242,7 +2239,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
@@ -2250,7 +2247,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="2:3" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.2">
@@ -2258,7 +2255,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="2:3" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.2">
@@ -2266,7 +2263,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="2:3" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.2">
@@ -2274,15 +2271,15 @@
         <v>4</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="2:3" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="B8" s="17" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">

</xml_diff>